<commit_message>
modify mt for algieba
</commit_message>
<xml_diff>
--- a/algieba/test/module_spec.xlsx
+++ b/algieba/test/module_spec.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="76">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -52,46 +52,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Account#show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#update</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#destroy</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#settle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#settle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#show</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#update</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#delete</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#settle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>条件</t>
     <rPh sb="0" eb="2">
       <t>ジョウケン</t>
@@ -100,10 +60,6 @@
   </si>
   <si>
     <t>1.0.0</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#show</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -234,14 +190,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Account#update</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Account#settle</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>interval: 'invalid_interval'</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -535,6 +483,34 @@
     <t>condition: {
   date: '1000-00-00'
 }</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.update</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.settle</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.show</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.destroy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.destroy</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Account.destroy</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1664,8 +1640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -1691,7 +1667,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
@@ -1705,14 +1681,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="44">
@@ -1723,14 +1699,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="44">
@@ -1741,14 +1717,14 @@
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="44">
@@ -1759,14 +1735,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="44">
@@ -1777,14 +1753,14 @@
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="57">
@@ -1795,14 +1771,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="57">
@@ -1810,17 +1786,17 @@
         <v>7</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="57">
@@ -1831,16 +1807,16 @@
         <v>6</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:7">
@@ -1851,14 +1827,14 @@
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>7</v>
+        <v>69</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="13" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="83">
@@ -1869,14 +1845,14 @@
         <v>5</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="83">
@@ -1887,14 +1863,14 @@
         <v>5</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="83">
@@ -1905,14 +1881,14 @@
         <v>5</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="83">
@@ -1923,14 +1899,14 @@
         <v>5</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="83">
@@ -1941,14 +1917,14 @@
         <v>5</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="122">
@@ -1959,14 +1935,14 @@
         <v>5</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="122">
@@ -1977,16 +1953,16 @@
         <v>5</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G18" s="13" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="70">
@@ -1997,14 +1973,14 @@
         <v>5</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="13" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="44">
@@ -2015,14 +1991,14 @@
         <v>5</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="44">
@@ -2033,14 +2009,14 @@
         <v>5</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F21" s="12"/>
       <c r="G21" s="13" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="44">
@@ -2051,14 +2027,14 @@
         <v>5</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="F22" s="12"/>
       <c r="G22" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="44">
@@ -2069,14 +2045,14 @@
         <v>5</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="F23" s="12"/>
       <c r="G23" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="44">
@@ -2087,14 +2063,14 @@
         <v>5</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F24" s="12"/>
       <c r="G24" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="2:7" ht="57">
@@ -2105,14 +2081,14 @@
         <v>5</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="F25" s="12"/>
       <c r="G25" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="2:7" ht="57">
@@ -2123,16 +2099,16 @@
         <v>5</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -2143,14 +2119,14 @@
         <v>5</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="13" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="2:7">
@@ -2161,14 +2137,14 @@
         <v>5</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F28" s="12"/>
       <c r="G28" s="13" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:7">
@@ -2179,14 +2155,14 @@
         <v>5</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="13" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="19" thickBot="1">
@@ -2197,14 +2173,14 @@
         <v>5</v>
       </c>
       <c r="D30" s="16" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F30" s="18"/>
       <c r="G30" s="19" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2223,8 +2199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2250,7 +2226,7 @@
         <v>4</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>2</v>
@@ -2264,14 +2240,14 @@
         <v>5</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F3" s="12"/>
       <c r="G3" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="44">
@@ -2282,14 +2258,14 @@
         <v>5</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>12</v>
+        <v>69</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F4" s="12"/>
       <c r="G4" s="13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="44">
@@ -2300,14 +2276,14 @@
         <v>5</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F5" s="12"/>
       <c r="G5" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="70">
@@ -2318,14 +2294,14 @@
         <v>5</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="13" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="83">
@@ -2336,14 +2312,14 @@
         <v>5</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F7" s="12"/>
       <c r="G7" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="83">
@@ -2354,14 +2330,14 @@
         <v>5</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>8</v>
+        <v>70</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="F8" s="12"/>
       <c r="G8" s="13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="83">
@@ -2372,14 +2348,14 @@
         <v>5</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="96">
@@ -2390,14 +2366,14 @@
         <v>5</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="F10" s="12"/>
       <c r="G10" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="83">
@@ -2408,14 +2384,14 @@
         <v>5</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="83">
@@ -2426,14 +2402,14 @@
         <v>5</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="83">
@@ -2444,14 +2420,14 @@
         <v>5</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:7" ht="109">
@@ -2459,17 +2435,17 @@
         <v>12</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="13" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:7" ht="70">
@@ -2480,14 +2456,14 @@
         <v>5</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="13" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="44">
@@ -2498,14 +2474,14 @@
         <v>5</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>15</v>
+        <v>74</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="13" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="44">
@@ -2516,14 +2492,14 @@
         <v>5</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="44">
@@ -2534,14 +2510,14 @@
         <v>5</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="13" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="70">
@@ -2552,14 +2528,14 @@
         <v>5</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="13" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:7">
@@ -2567,17 +2543,17 @@
         <v>18</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F20" s="12"/>
       <c r="G20" s="13" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="19" thickBot="1">
@@ -2588,14 +2564,14 @@
         <v>5</v>
       </c>
       <c r="D21" s="21" t="s">
-        <v>16</v>
+        <v>71</v>
       </c>
       <c r="E21" s="22" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="F21" s="23"/>
       <c r="G21" s="24" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>